<commit_message>
[Add] Npc Model 일부 추가 - KKH
</commit_message>
<xml_diff>
--- a/Assets/ExcelFile/ServeQuestDB.xlsx
+++ b/Assets/ExcelFile/ServeQuestDB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\unityhub\storage\FinalProject\Assets\ExcelFile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7068728C-C11D-4336-9138-B662AE09DE7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C910D83-04BE-4260-8F93-20F7A84ED45B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B3A9DE6C-8FB1-4993-A516-889844C681F3}"/>
   </bookViews>
@@ -33,8 +33,173 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>kkh</author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{43C44C8B-195F-4884-815D-BBE3B1417747}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>kkh:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+1.</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t xml:space="preserve">마법사
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>100.</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t xml:space="preserve">대장장이
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>200.</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t xml:space="preserve">요리사
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>300</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t xml:space="preserve">잡화
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>400</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t xml:space="preserve">여관
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>500</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t xml:space="preserve">검술
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>9999</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t xml:space="preserve">미정
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
   <si>
     <t>Reword</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -52,14 +217,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>도토리수집</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>도토리ㅏ가져와</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -112,55 +269,91 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>도토리가필요해,ㅇㅇㅇ</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>목검가져오기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>목검 rr</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>목검가꼬와,빨리ㅏ</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>고마워 이건 보답이야</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>테스트중</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>포션 가져가기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>포션을 가져가자</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>포션이 필요한데,가져다줄래??</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ㅋㅋ감사</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>teset</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>test</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ss</t>
+    <t>땔감이 필요해</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>땔감을 가져다주자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>많이 못보던 사람이네??,지금 혹시 할일이 없다면 내 부탁좀 들어주지 않을래?,나는 대장간을 운영하는 대장장이인데,화로에 지필 나무가 많이 필요해,마을 밖에 초원에서 땔감좀 구해주면 나한테는 필요없는 물건을 줄게,몸 조심해!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>생각보다 빨리 구해왔네,도와줘서 고마워,이건 옛날에 내가 모험가일때 쓰던 포션인데,더 이상 모험을 하지않으니까 이건 주는게 맞는거같아,부디 잘써줘</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>제작에 대하여[튜토리얼]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>튜토리얼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>또 보는구나!, 혹시 이제 앞으로 모험을 나가게되면 수많은 재료들을 볼 수 있을텐데,그걸 그냥 그대로 두기보단 나에게 가져오는게 어때?,내가 쓸만하게 가공해줄 수 있으니까,그럼 제작에 대해 알려줄테니,옆집에 상점관리인에게 나무검 레시피를 하나 구해와</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>제작은 레시피와 레시피에 적혀진 갖가지 재료들이 꼭 필요해, 대화가 끝나면 나에게 제작을 해보지 않을래?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아저씨의 고민</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몬스터사냥임</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>요 며칠동안 잠을 통 자지못했어, 혹시 바쁘지 않다면 내 부탁을 좀 들어줄래??,우리 집 앞에 몬스터들이 내 잠을 방해해,걔내들을 좀 처리해줘</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>부탁을 들어줘서 고마워,혹시 나중에 또 바쁘지않으면 들어주겠어??,나중에 보자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아저씨의 고민2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>또 보는구나!, 이번에도 너의 도움이 필요해, 이번엔 저번보다 개채수가 많이 늘어난거 같아, 처리하게 되면 알려줘</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>매번 도움을 줘서 고마워, 나중에 또 보자!,이건 내 답례야</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아저씨의 고민3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몬스터사냥임 최종</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>내 불면증이 날이 갈 수록 악화 되가고있어,이건 몬스터의 문제가 아닌거 같아, 혹시 상점이나 너가 따듯한 스프를 가지고 있다면 혹시 가져다 주지않을래?,난 피곤해서 움직일 수 가없어 미안해</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>정말 고마워,덕분에 오늘은 푹 잘 수 있을것만 같아,매번 부탁을 들어줘서 고마워</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>야영의 대하여[튜토리얼]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>안녕! 처음보는 모험가네??,혹시 야영에 대해 알고있어?,혹시 한번도 야영을 해보지 못했다면 내 부탁들 좀 들어줄래??,간이 야영지로 사용할 짚과 나무를 좀 구해다줘!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>용케 빨리 잘 모아왔구나!, 이제그럼 야영에 대해 설명해줄게, 야영이란 마을 외 지역에서 간단하게 시간을 보낼 수 있는 행위를 뜻해!,너에게 간이 야영키트를 줬으니 한번 사용해보도록 해봐!, 야영방법은 [T]를 눌르면 자연스럽게 알게될거야!, 그럼 나중에보자</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -168,7 +361,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -183,6 +376,26 @@
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="돋움"/>
+      <family val="3"/>
+      <charset val="129"/>
     </font>
   </fonts>
   <fills count="2">
@@ -527,11 +740,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CFA5ABC-5119-4986-967B-E769D16FD73A}">
-  <dimension ref="A1:Q5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CFA5ABC-5119-4986-967B-E769D16FD73A}">
+  <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -545,43 +758,43 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>0</v>
@@ -601,22 +814,22 @@
         <v>10001</v>
       </c>
       <c r="B2" s="1">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="C2" s="1">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="F2">
-        <v>3000</v>
+        <v>2001</v>
       </c>
       <c r="G2" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H2" s="1">
         <v>0</v>
@@ -625,19 +838,19 @@
         <v>0</v>
       </c>
       <c r="J2" s="1">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="K2" s="1">
         <v>0</v>
       </c>
       <c r="L2" s="1">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="M2" s="1">
         <v>0</v>
       </c>
       <c r="N2">
-        <v>3000</v>
+        <v>10100000</v>
       </c>
       <c r="O2">
         <v>0</v>
@@ -646,7 +859,7 @@
         <v>19</v>
       </c>
       <c r="Q2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
@@ -657,101 +870,77 @@
         <v>100</v>
       </c>
       <c r="C3" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3">
-        <v>10010000</v>
+        <v>22</v>
+      </c>
+      <c r="F3" s="1">
+        <v>10110000</v>
       </c>
       <c r="G3" s="1">
         <v>1</v>
       </c>
-      <c r="H3" s="1">
-        <v>0</v>
-      </c>
-      <c r="I3" s="1">
-        <v>0</v>
-      </c>
-      <c r="J3" s="1">
-        <v>-1</v>
-      </c>
-      <c r="K3" s="1">
-        <v>0</v>
-      </c>
-      <c r="L3" s="1">
-        <v>1</v>
-      </c>
-      <c r="M3" s="1">
-        <v>0</v>
-      </c>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
       <c r="N3">
-        <v>3000</v>
+        <v>10110000</v>
       </c>
       <c r="O3">
         <v>0</v>
       </c>
       <c r="P3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="Q3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>10003</v>
       </c>
-      <c r="B4">
-        <v>1000</v>
-      </c>
-      <c r="C4">
+      <c r="B4" s="1">
+        <v>1200</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1">
         <v>1</v>
       </c>
-      <c r="D4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4">
-        <v>10100000</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>-1</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>-1</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4">
-        <v>10001000</v>
-      </c>
-      <c r="O4">
-        <v>0</v>
-      </c>
-      <c r="P4" t="s">
+      <c r="K4" s="1">
+        <v>5</v>
+      </c>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1">
+        <v>0</v>
+      </c>
+      <c r="O4" s="1">
+        <v>0</v>
+      </c>
+      <c r="P4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="Q4" s="1" t="s">
         <v>28</v>
       </c>
     </row>
@@ -760,57 +949,125 @@
         <v>10004</v>
       </c>
       <c r="B5" s="1">
-        <v>100</v>
-      </c>
-      <c r="C5">
+        <v>1200</v>
+      </c>
+      <c r="C5" s="1">
         <v>2</v>
       </c>
       <c r="D5" t="s">
         <v>29</v>
       </c>
-      <c r="E5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5" s="1">
-        <v>0</v>
-      </c>
-      <c r="H5" s="1">
-        <v>0</v>
-      </c>
-      <c r="I5" s="1">
-        <v>0</v>
-      </c>
+      <c r="E5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
       <c r="J5" s="1">
         <v>1</v>
       </c>
       <c r="K5" s="1">
+        <v>5</v>
+      </c>
+      <c r="L5" s="1">
+        <v>2</v>
+      </c>
+      <c r="M5" s="1">
+        <v>5</v>
+      </c>
+      <c r="N5" s="1">
+        <v>0</v>
+      </c>
+      <c r="O5" s="1">
+        <v>0</v>
+      </c>
+      <c r="P5" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>10005</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1200</v>
+      </c>
+      <c r="C6" s="1">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J6" s="1">
         <v>1</v>
       </c>
-      <c r="L5" s="1">
-        <v>-1</v>
-      </c>
-      <c r="M5" s="1">
-        <v>0</v>
-      </c>
-      <c r="N5" s="1">
-        <v>0</v>
-      </c>
-      <c r="O5" s="1">
-        <v>0</v>
-      </c>
-      <c r="P5" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q5">
-        <v>123</v>
+      <c r="K6" s="1">
+        <v>10</v>
+      </c>
+      <c r="L6">
+        <v>2</v>
+      </c>
+      <c r="M6">
+        <v>10</v>
+      </c>
+      <c r="N6" s="1">
+        <v>0</v>
+      </c>
+      <c r="O6" s="1">
+        <v>0</v>
+      </c>
+      <c r="P6" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>10006</v>
+      </c>
+      <c r="B7">
+        <v>400</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7">
+        <v>2003</v>
+      </c>
+      <c r="G7" s="1">
+        <v>3</v>
+      </c>
+      <c r="H7">
+        <v>2001</v>
+      </c>
+      <c r="I7" s="1">
+        <v>3</v>
+      </c>
+      <c r="P7" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[Add] Npc Model 일부 추가 - KKH (#60)
</commit_message>
<xml_diff>
--- a/Assets/ExcelFile/ServeQuestDB.xlsx
+++ b/Assets/ExcelFile/ServeQuestDB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\unityhub\storage\FinalProject\Assets\ExcelFile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7068728C-C11D-4336-9138-B662AE09DE7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C910D83-04BE-4260-8F93-20F7A84ED45B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B3A9DE6C-8FB1-4993-A516-889844C681F3}"/>
   </bookViews>
@@ -33,8 +33,173 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>kkh</author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{43C44C8B-195F-4884-815D-BBE3B1417747}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>kkh:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+1.</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t xml:space="preserve">마법사
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>100.</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t xml:space="preserve">대장장이
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>200.</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t xml:space="preserve">요리사
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>300</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t xml:space="preserve">잡화
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>400</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t xml:space="preserve">여관
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>500</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t xml:space="preserve">검술
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>9999</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t xml:space="preserve">미정
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
   <si>
     <t>Reword</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -52,14 +217,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>도토리수집</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>도토리ㅏ가져와</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -112,55 +269,91 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>도토리가필요해,ㅇㅇㅇ</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>목검가져오기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>목검 rr</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>목검가꼬와,빨리ㅏ</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>고마워 이건 보답이야</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>테스트중</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>포션 가져가기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>포션을 가져가자</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>포션이 필요한데,가져다줄래??</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ㅋㅋ감사</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>teset</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>test</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ss</t>
+    <t>땔감이 필요해</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>땔감을 가져다주자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>많이 못보던 사람이네??,지금 혹시 할일이 없다면 내 부탁좀 들어주지 않을래?,나는 대장간을 운영하는 대장장이인데,화로에 지필 나무가 많이 필요해,마을 밖에 초원에서 땔감좀 구해주면 나한테는 필요없는 물건을 줄게,몸 조심해!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>생각보다 빨리 구해왔네,도와줘서 고마워,이건 옛날에 내가 모험가일때 쓰던 포션인데,더 이상 모험을 하지않으니까 이건 주는게 맞는거같아,부디 잘써줘</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>제작에 대하여[튜토리얼]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>튜토리얼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>또 보는구나!, 혹시 이제 앞으로 모험을 나가게되면 수많은 재료들을 볼 수 있을텐데,그걸 그냥 그대로 두기보단 나에게 가져오는게 어때?,내가 쓸만하게 가공해줄 수 있으니까,그럼 제작에 대해 알려줄테니,옆집에 상점관리인에게 나무검 레시피를 하나 구해와</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>제작은 레시피와 레시피에 적혀진 갖가지 재료들이 꼭 필요해, 대화가 끝나면 나에게 제작을 해보지 않을래?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아저씨의 고민</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몬스터사냥임</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>요 며칠동안 잠을 통 자지못했어, 혹시 바쁘지 않다면 내 부탁을 좀 들어줄래??,우리 집 앞에 몬스터들이 내 잠을 방해해,걔내들을 좀 처리해줘</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>부탁을 들어줘서 고마워,혹시 나중에 또 바쁘지않으면 들어주겠어??,나중에 보자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아저씨의 고민2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>또 보는구나!, 이번에도 너의 도움이 필요해, 이번엔 저번보다 개채수가 많이 늘어난거 같아, 처리하게 되면 알려줘</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>매번 도움을 줘서 고마워, 나중에 또 보자!,이건 내 답례야</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아저씨의 고민3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몬스터사냥임 최종</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>내 불면증이 날이 갈 수록 악화 되가고있어,이건 몬스터의 문제가 아닌거 같아, 혹시 상점이나 너가 따듯한 스프를 가지고 있다면 혹시 가져다 주지않을래?,난 피곤해서 움직일 수 가없어 미안해</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>정말 고마워,덕분에 오늘은 푹 잘 수 있을것만 같아,매번 부탁을 들어줘서 고마워</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>야영의 대하여[튜토리얼]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>안녕! 처음보는 모험가네??,혹시 야영에 대해 알고있어?,혹시 한번도 야영을 해보지 못했다면 내 부탁들 좀 들어줄래??,간이 야영지로 사용할 짚과 나무를 좀 구해다줘!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>용케 빨리 잘 모아왔구나!, 이제그럼 야영에 대해 설명해줄게, 야영이란 마을 외 지역에서 간단하게 시간을 보낼 수 있는 행위를 뜻해!,너에게 간이 야영키트를 줬으니 한번 사용해보도록 해봐!, 야영방법은 [T]를 눌르면 자연스럽게 알게될거야!, 그럼 나중에보자</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -168,7 +361,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -183,6 +376,26 @@
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="돋움"/>
+      <family val="3"/>
+      <charset val="129"/>
     </font>
   </fonts>
   <fills count="2">
@@ -527,11 +740,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CFA5ABC-5119-4986-967B-E769D16FD73A}">
-  <dimension ref="A1:Q5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CFA5ABC-5119-4986-967B-E769D16FD73A}">
+  <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -545,43 +758,43 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>0</v>
@@ -601,22 +814,22 @@
         <v>10001</v>
       </c>
       <c r="B2" s="1">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="C2" s="1">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="F2">
-        <v>3000</v>
+        <v>2001</v>
       </c>
       <c r="G2" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H2" s="1">
         <v>0</v>
@@ -625,19 +838,19 @@
         <v>0</v>
       </c>
       <c r="J2" s="1">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="K2" s="1">
         <v>0</v>
       </c>
       <c r="L2" s="1">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="M2" s="1">
         <v>0</v>
       </c>
       <c r="N2">
-        <v>3000</v>
+        <v>10100000</v>
       </c>
       <c r="O2">
         <v>0</v>
@@ -646,7 +859,7 @@
         <v>19</v>
       </c>
       <c r="Q2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
@@ -657,101 +870,77 @@
         <v>100</v>
       </c>
       <c r="C3" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3">
-        <v>10010000</v>
+        <v>22</v>
+      </c>
+      <c r="F3" s="1">
+        <v>10110000</v>
       </c>
       <c r="G3" s="1">
         <v>1</v>
       </c>
-      <c r="H3" s="1">
-        <v>0</v>
-      </c>
-      <c r="I3" s="1">
-        <v>0</v>
-      </c>
-      <c r="J3" s="1">
-        <v>-1</v>
-      </c>
-      <c r="K3" s="1">
-        <v>0</v>
-      </c>
-      <c r="L3" s="1">
-        <v>1</v>
-      </c>
-      <c r="M3" s="1">
-        <v>0</v>
-      </c>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
       <c r="N3">
-        <v>3000</v>
+        <v>10110000</v>
       </c>
       <c r="O3">
         <v>0</v>
       </c>
       <c r="P3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="Q3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>10003</v>
       </c>
-      <c r="B4">
-        <v>1000</v>
-      </c>
-      <c r="C4">
+      <c r="B4" s="1">
+        <v>1200</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1">
         <v>1</v>
       </c>
-      <c r="D4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4">
-        <v>10100000</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>-1</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>-1</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4">
-        <v>10001000</v>
-      </c>
-      <c r="O4">
-        <v>0</v>
-      </c>
-      <c r="P4" t="s">
+      <c r="K4" s="1">
+        <v>5</v>
+      </c>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1">
+        <v>0</v>
+      </c>
+      <c r="O4" s="1">
+        <v>0</v>
+      </c>
+      <c r="P4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="Q4" s="1" t="s">
         <v>28</v>
       </c>
     </row>
@@ -760,57 +949,125 @@
         <v>10004</v>
       </c>
       <c r="B5" s="1">
-        <v>100</v>
-      </c>
-      <c r="C5">
+        <v>1200</v>
+      </c>
+      <c r="C5" s="1">
         <v>2</v>
       </c>
       <c r="D5" t="s">
         <v>29</v>
       </c>
-      <c r="E5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5" s="1">
-        <v>0</v>
-      </c>
-      <c r="H5" s="1">
-        <v>0</v>
-      </c>
-      <c r="I5" s="1">
-        <v>0</v>
-      </c>
+      <c r="E5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
       <c r="J5" s="1">
         <v>1</v>
       </c>
       <c r="K5" s="1">
+        <v>5</v>
+      </c>
+      <c r="L5" s="1">
+        <v>2</v>
+      </c>
+      <c r="M5" s="1">
+        <v>5</v>
+      </c>
+      <c r="N5" s="1">
+        <v>0</v>
+      </c>
+      <c r="O5" s="1">
+        <v>0</v>
+      </c>
+      <c r="P5" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>10005</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1200</v>
+      </c>
+      <c r="C6" s="1">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J6" s="1">
         <v>1</v>
       </c>
-      <c r="L5" s="1">
-        <v>-1</v>
-      </c>
-      <c r="M5" s="1">
-        <v>0</v>
-      </c>
-      <c r="N5" s="1">
-        <v>0</v>
-      </c>
-      <c r="O5" s="1">
-        <v>0</v>
-      </c>
-      <c r="P5" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q5">
-        <v>123</v>
+      <c r="K6" s="1">
+        <v>10</v>
+      </c>
+      <c r="L6">
+        <v>2</v>
+      </c>
+      <c r="M6">
+        <v>10</v>
+      </c>
+      <c r="N6" s="1">
+        <v>0</v>
+      </c>
+      <c r="O6" s="1">
+        <v>0</v>
+      </c>
+      <c r="P6" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>10006</v>
+      </c>
+      <c r="B7">
+        <v>400</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7">
+        <v>2003</v>
+      </c>
+      <c r="G7" s="1">
+        <v>3</v>
+      </c>
+      <c r="H7">
+        <v>2001</v>
+      </c>
+      <c r="I7" s="1">
+        <v>3</v>
+      </c>
+      <c r="P7" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>